<commit_message>
changed some components to tht for assy
</commit_message>
<xml_diff>
--- a/DOC/Temporizador_V8_THT.xlsx
+++ b/DOC/Temporizador_V8_THT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo\Desktop\GitHub Repos\TemporizadorAC\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D7BFA2-1E73-4A8F-A5FB-CCFB63B3854D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BDB96E-25A3-4257-820D-171CCEE5E2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3823098C-5F4A-4E09-BFE5-BB9307522169}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="80">
   <si>
     <t>Comment</t>
   </si>
@@ -59,15 +59,9 @@
     <t>10uF/50V</t>
   </si>
   <si>
-    <t>C440198</t>
-  </si>
-  <si>
     <t>CADJ_POW</t>
   </si>
   <si>
-    <t>0805-CAP-TDK</t>
-  </si>
-  <si>
     <t>1N5349</t>
   </si>
   <si>
@@ -83,27 +77,12 @@
     <t>100uFx63V</t>
   </si>
   <si>
-    <t>C178628</t>
-  </si>
-  <si>
     <t>C5_POW</t>
   </si>
   <si>
-    <t>DIA10X10.2-CAP-SMD</t>
-  </si>
-  <si>
-    <t>4.7uF/25V</t>
-  </si>
-  <si>
-    <t>C1779</t>
-  </si>
-  <si>
     <t>CB1_UC_INT</t>
   </si>
   <si>
-    <t>0805-RES-PANASONIC</t>
-  </si>
-  <si>
     <t>0.1uF</t>
   </si>
   <si>
@@ -113,27 +92,18 @@
     <t>0.33uF</t>
   </si>
   <si>
-    <t>C3_POW</t>
-  </si>
-  <si>
     <t>1N4007</t>
   </si>
   <si>
     <t>D1_FAN, D1_HEAT, D1_LIMIT, D1_POW, D1_VACUUM, D1_VALVE, D2_POW, D3_POW, D4_POW</t>
   </si>
   <si>
-    <t>DO-214AC-SMA</t>
-  </si>
-  <si>
     <t>1N4148</t>
   </si>
   <si>
     <t>D1_ACT_INT, D2_ACT_INT</t>
   </si>
   <si>
-    <t>SOD-123</t>
-  </si>
-  <si>
     <t>3K3/1%</t>
   </si>
   <si>
@@ -191,18 +161,6 @@
     <t>DBS</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>DL1_ACT_INT</t>
-  </si>
-  <si>
-    <t>LED-5MM - BI</t>
-  </si>
-  <si>
-    <t>MMSZ18T1G</t>
-  </si>
-  <si>
     <t>D2_FAN, D2_HEAT, D2_LIMIT, D2_VACUUM, D2_VALVE</t>
   </si>
   <si>
@@ -215,15 +173,9 @@
     <t>ST-TSSOP-20 - STM32F031F6P7</t>
   </si>
   <si>
-    <t>TLP521-1</t>
-  </si>
-  <si>
     <t>U1_FAN, U1_HEAT, U1_LIMIT, U1_VACUUM, U1_VALVE</t>
   </si>
   <si>
-    <t>SMD-4P</t>
-  </si>
-  <si>
     <t>ULN2003</t>
   </si>
   <si>
@@ -243,6 +195,90 @@
   </si>
   <si>
     <t>C5377</t>
+  </si>
+  <si>
+    <t>C69256</t>
+  </si>
+  <si>
+    <t>TLP521-1GB</t>
+  </si>
+  <si>
+    <t>C391339</t>
+  </si>
+  <si>
+    <t>1N4746A-G</t>
+  </si>
+  <si>
+    <t>DO-41G</t>
+  </si>
+  <si>
+    <t>C3033995</t>
+  </si>
+  <si>
+    <t>DO-41</t>
+  </si>
+  <si>
+    <t>C24497</t>
+  </si>
+  <si>
+    <t>1206-CAP-TDK</t>
+  </si>
+  <si>
+    <t>C2761750</t>
+  </si>
+  <si>
+    <t>CAP-200</t>
+  </si>
+  <si>
+    <t>C258182</t>
+  </si>
+  <si>
+    <t>DO-35</t>
+  </si>
+  <si>
+    <t>C2940713</t>
+  </si>
+  <si>
+    <t>CAP-100RP</t>
+  </si>
+  <si>
+    <t>C165651</t>
+  </si>
+  <si>
+    <t>CAP-200RP</t>
+  </si>
+  <si>
+    <t>4.7uF/50V</t>
+  </si>
+  <si>
+    <t>C29823</t>
+  </si>
+  <si>
+    <t>C17936</t>
+  </si>
+  <si>
+    <t>1206-RES-PANASONIC</t>
+  </si>
+  <si>
+    <t>RES400</t>
+  </si>
+  <si>
+    <t>C119315</t>
+  </si>
+  <si>
+    <t>C119310</t>
+  </si>
+  <si>
+    <t>C119345</t>
+  </si>
+  <si>
+    <t>C173035</t>
+  </si>
+  <si>
+    <t>C119335</t>
+  </si>
+  <si>
+    <t>DIP4</t>
   </si>
 </sst>
 </file>
@@ -305,15 +341,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693F7A0C-05E1-4B13-8262-C54E2361998D}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,366 +678,375 @@
     <col min="3" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="B9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2" t="s">
+      <c r="B10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="D10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2" t="s">
+      <c r="B11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="D11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2" t="s">
+      <c r="B12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="B13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2" t="s">
+      <c r="D13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1">
+      <c r="B15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1">
+    <row r="18" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="1">
+    <row r="20" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="5" t="s">
+    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="B22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="6">
+      <c r="E22" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>